<commit_message>
add new check for user validation
</commit_message>
<xml_diff>
--- a/data/credentials.xlsx
+++ b/data/credentials.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Username</t>
   </si>
@@ -56,12 +56,6 @@
   </si>
   <si>
     <t>anna1983</t>
-  </si>
-  <si>
-    <t>arushanyan.natali@mail.ru</t>
-  </si>
-  <si>
-    <t>natali1996</t>
   </si>
   <si>
     <t>ashotstepanyan@hotmail.com</t>
@@ -81,7 +75,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,12 +107,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -170,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -185,9 +173,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -501,15 +486,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="40.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="32.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="38.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="40.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="32.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="38.71928571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -589,48 +574,39 @@
       <c r="C8" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="A9" s="5"/>
+      <c r="B9" s="6"/>
       <c r="C9" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
       <c r="C11" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="A13" s="4"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="4"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="4"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="4"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>